<commit_message>
feat: API for add students into DB (undone)
</commit_message>
<xml_diff>
--- a/SD/FormDesign.xlsx
+++ b/SD/FormDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nana\SE_2024_fall\git\ratingForm\SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B87EB7-36FE-4A0F-A70D-1BE5E5F0CDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE230CFD-83CA-4028-A4FC-45C906B97E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B524B075-65A8-4B41-B81D-ADC7B61B9386}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>學號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Table: 總修課學生</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>班別(在職/日間)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -351,6 +347,42 @@
   </si>
   <si>
     <t>Table: GradeEntity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table: ReviewerEntity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>報告週次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gradeList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[90, 88.2, …, 94.13]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[90, 93.76, …, 94.13]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table: StudentEntity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -853,7 +885,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1091,13 +1123,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1495,10 +1533,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5008D-195E-6E41-9403-DEB5B043E7BA}">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
@@ -1514,14 +1552,14 @@
     <col min="12" max="13" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" thickBot="1">
+    <row r="1" spans="2:12" ht="17.25" thickBot="1">
       <c r="B1" s="59" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12">
       <c r="B2" s="52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -1534,12 +1572,12 @@
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="2:12">
       <c r="B3" s="55" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="60"/>
       <c r="E3" s="60"/>
@@ -1551,12 +1589,12 @@
       <c r="K3" s="60"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" thickBot="1">
+    <row r="4" spans="2:12" ht="17.25" thickBot="1">
       <c r="B4" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="57"/>
       <c r="E4" s="57"/>
@@ -1568,27 +1606,27 @@
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" s="61" customFormat="1">
+    <row r="5" spans="2:12" s="61" customFormat="1">
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
       <c r="J5" s="62"/>
       <c r="K5" s="62"/>
       <c r="L5" s="62"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" thickBot="1">
+    <row r="6" spans="2:12" ht="17.25" thickBot="1">
       <c r="B6" s="51" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="26" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
       <c r="E7" s="28"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="2:12">
       <c r="B8" s="29" t="s">
         <v>0</v>
       </c>
@@ -1599,563 +1637,576 @@
         <v>2</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>48</v>
-      </c>
       <c r="E9" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
       <c r="B11" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="17.25" thickBot="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="17.25" thickBot="1">
       <c r="B12" s="33" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="83" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="60" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" ht="17.25" thickBot="1">
-      <c r="D13" s="25"/>
-      <c r="I13" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="B15" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="D16" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" s="83" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="17.25" thickBot="1">
+      <c r="D18" s="25"/>
+      <c r="I18" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16" s="79" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="13" t="s">
+      <c r="F20" s="30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="14">
+      <c r="E21" s="14">
         <v>1</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="31"/>
-    </row>
-    <row r="17" spans="1:8" ht="17.25" thickBot="1">
-      <c r="B17" s="80" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="37" t="s">
+      <c r="F21" s="74"/>
+    </row>
+    <row r="22" spans="1:9" ht="17.25" thickBot="1">
+      <c r="B22" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="34">
+      <c r="E22" s="34">
         <v>2</v>
       </c>
-      <c r="E17" s="75"/>
-    </row>
-    <row r="18" spans="1:8" s="61" customFormat="1"/>
-    <row r="19" spans="1:8">
-      <c r="A19" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="77" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="B20" s="2" t="s">
+      <c r="F22" s="75"/>
+    </row>
+    <row r="23" spans="1:9" s="61" customFormat="1"/>
+    <row r="24" spans="1:9">
+      <c r="A24" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="77" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="B21" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="71" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="81" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="B22" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="73" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="71"/>
-      <c r="G22" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="81" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="B26" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="66" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="73" t="s">
+      <c r="E26" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="F26" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" s="81" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="B27" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="73" t="s">
-        <v>64</v>
-      </c>
+      <c r="E27" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="71"/>
       <c r="G27" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27" s="81" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="71" customFormat="1">
-      <c r="D28" s="72"/>
-    </row>
-    <row r="29" spans="1:8">
+        <v>55</v>
+      </c>
+      <c r="H27" s="79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="B32" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="71" customFormat="1">
+      <c r="D33" s="72"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="B31" t="s">
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C36" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D36" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="71">
+      <c r="E36" s="71">
         <v>1</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="B32" t="s">
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="B37" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="70" t="s">
+      <c r="C37" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D37" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="71">
+      <c r="E37" s="71">
         <v>2</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="B33" t="s">
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="70" t="s">
+      <c r="C38" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D38" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="71">
+      <c r="E38" s="71">
         <v>1</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="B34" t="s">
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C39" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D39" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="71">
+      <c r="E39" s="71">
         <v>2</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-    </row>
-    <row r="35" spans="1:13" s="61" customFormat="1">
-      <c r="D35" s="63"/>
-    </row>
-    <row r="36" spans="1:13" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B36" t="s">
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+    </row>
+    <row r="40" spans="1:13" s="61" customFormat="1">
+      <c r="D40" s="63"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.95" customHeight="1" thickBot="1">
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="7"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="B43" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="B44" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="62">
+        <v>1</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="14">
+        <v>90</v>
+      </c>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="18"/>
+    </row>
+    <row r="45" spans="1:13" ht="17.25" thickBot="1">
+      <c r="B45" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="67">
+        <v>1</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="21">
+        <v>80</v>
+      </c>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="24"/>
+    </row>
+    <row r="46" spans="1:13" s="61" customFormat="1"/>
+    <row r="47" spans="1:13" ht="17.25" thickBot="1">
+      <c r="B47" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="7"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="B38" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="B39" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="62">
-        <v>1</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G39" s="14">
-        <v>90</v>
-      </c>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="62"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="18"/>
-    </row>
-    <row r="40" spans="1:13" ht="17.25" thickBot="1">
-      <c r="B40" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="67">
-        <v>1</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G40" s="21">
-        <v>80</v>
-      </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="67"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="24"/>
-    </row>
-    <row r="41" spans="1:13" s="61" customFormat="1"/>
-    <row r="42" spans="1:13" ht="17.25" thickBot="1">
-      <c r="B42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="B43" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="40"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="B44" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="B45" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="17">
-        <v>88.99</v>
-      </c>
-      <c r="D45" s="81" t="s">
-        <v>79</v>
-      </c>
-      <c r="E45" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="17.25" thickBot="1">
-      <c r="B46" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="46">
-        <v>87.24</v>
-      </c>
-      <c r="D46" s="81" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="17.25" thickBot="1"/>
+    </row>
     <row r="48" spans="1:13">
       <c r="B48" s="38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="39"/>
-      <c r="D48" s="40"/>
-    </row>
-    <row r="49" spans="2:4">
+      <c r="D48" s="39"/>
+      <c r="E48" s="40"/>
+    </row>
+    <row r="49" spans="2:5">
       <c r="B49" s="41" t="s">
         <v>0</v>
       </c>
@@ -2163,41 +2214,91 @@
         <v>3</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="17">
+        <v>88.99</v>
+      </c>
+      <c r="D50" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B51" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="46">
+        <v>87.24</v>
+      </c>
+      <c r="D51" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="17.25" thickBot="1"/>
+    <row r="53" spans="2:5">
+      <c r="B53" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="39"/>
+      <c r="D53" s="40"/>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C55" s="16">
         <v>86</v>
       </c>
-      <c r="D50" s="81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="17.25" thickBot="1">
-      <c r="B51" s="49" t="s">
+      <c r="D55" s="79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B56" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="50">
+      <c r="C56" s="50">
         <v>93</v>
       </c>
-      <c r="D51" s="81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" s="61" customFormat="1"/>
+      <c r="D56" s="79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" s="61" customFormat="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{50A1BB5F-741E-AA42-991C-731854855B86}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{C01AE86F-D73C-9F4C-B7B8-5FA80445DB3E}"/>
-    <hyperlink ref="E26" r:id="rId3" xr:uid="{E1D17CF0-C9DF-4582-B5D7-311279FF79CC}"/>
-    <hyperlink ref="E27" r:id="rId4" xr:uid="{A9F37BA5-1C09-4282-80DA-4BB25919CF35}"/>
-    <hyperlink ref="D21" r:id="rId5" xr:uid="{5EFBF140-85EA-44D8-AB66-8559CC8F9FA6}"/>
-    <hyperlink ref="D22" r:id="rId6" xr:uid="{2956C5A9-C70B-4ED2-B816-21B2CDC2D1D7}"/>
+    <hyperlink ref="E31" r:id="rId3" xr:uid="{E1D17CF0-C9DF-4582-B5D7-311279FF79CC}"/>
+    <hyperlink ref="E32" r:id="rId4" xr:uid="{A9F37BA5-1C09-4282-80DA-4BB25919CF35}"/>
+    <hyperlink ref="D26" r:id="rId5" xr:uid="{5EFBF140-85EA-44D8-AB66-8559CC8F9FA6}"/>
+    <hyperlink ref="D27" r:id="rId6" xr:uid="{2956C5A9-C70B-4ED2-B816-21B2CDC2D1D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>